<commit_message>
What's even the point of this repo
</commit_message>
<xml_diff>
--- a/Task logs 2.xlsx
+++ b/Task logs 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3HanbieDir\Hanbie Laboratories\Programs\Programming\Unity\Games\Flammable Blood\Flammable_Blood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39492B73-00DA-4547-926C-0E852A95E59D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E58C56C-527E-49BA-82BA-8A8A8E54681A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F928562-C088-4B7D-BD3F-8CA739E95BAB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Task logs V 2.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,10 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hours spent:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Estimate hours:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,6 +102,30 @@
   </si>
   <si>
     <t>Inventory: item stats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Estimated percentage:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display debug cmd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RainSFX Intro vol/pan control, Intro start anim disable, intro level design, enemy stats update, enemy AI update etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hours spent (day):</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hours spent (task):</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -256,13 +276,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -311,15 +359,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -328,6 +370,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,17 +718,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8CE429-F9AD-4ED1-8951-0ED433F08095}">
-  <dimension ref="F1:O101"/>
+  <dimension ref="E1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="9" style="1"/>
     <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="10.375" style="24" customWidth="1"/>
     <col min="7" max="7" width="23" style="15" customWidth="1"/>
     <col min="8" max="8" width="18.5" style="15" customWidth="1"/>
     <col min="9" max="10" width="9" style="15"/>
@@ -661,32 +736,32 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:15">
-      <c r="F1" s="10"/>
+    <row r="1" spans="5:21">
+      <c r="F1" s="20"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="6:15">
-      <c r="F2" s="10"/>
+    <row r="2" spans="5:21">
+      <c r="F2" s="20"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="6:15">
-      <c r="F3" s="10"/>
+    <row r="3" spans="5:21">
+      <c r="F3" s="20"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="6:15" ht="35.25" customHeight="1">
-      <c r="F4" s="10"/>
+    <row r="4" spans="5:21" ht="35.25" customHeight="1">
+      <c r="F4" s="20"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -699,58 +774,74 @@
       <c r="N4" s="8"/>
       <c r="O4" s="1">
         <f xml:space="preserve"> SUM(J8:J100)</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="5" spans="6:15" ht="33" customHeight="1">
-      <c r="F5" s="10"/>
-      <c r="G5" s="21" t="s">
+        <v>8.7000000000000011</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="25">
+        <f>O5/O4</f>
+        <v>0.17241379310344826</v>
+      </c>
+      <c r="U4" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="5:21" ht="33" customHeight="1">
+      <c r="F5" s="20"/>
+      <c r="G5" s="19" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="17"/>
+      <c r="M5" s="16"/>
       <c r="O5" s="1">
-        <f>SUM(K8:K100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="6:15" ht="15" thickBot="1">
-      <c r="F6" s="10"/>
+        <f>SUM(E8:E100)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="5:21" ht="15.75" thickBot="1">
+      <c r="F6" s="20"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="12"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="6:15" s="2" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
-      <c r="F7" s="18" t="s">
+    <row r="7" spans="5:21" s="2" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
+      <c r="E7" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="20" t="s">
+      <c r="J7" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F8" s="16">
-        <v>43837</v>
+      <c r="K7" s="27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E8" s="30"/>
+      <c r="F8" s="21">
+        <v>44013</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>7</v>
@@ -759,60 +850,78 @@
         <v>6</v>
       </c>
       <c r="I8" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="13">
         <v>0.5</v>
       </c>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="K8" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="5:21" s="2" customFormat="1" ht="72.75" customHeight="1">
+      <c r="E9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="21">
+        <v>44044</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="13">
         <v>0.5</v>
       </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F10" s="13"/>
+      <c r="K9" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E10" s="4"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="13">
         <v>0.7</v>
       </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F11" s="13"/>
+      <c r="K10" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E11" s="4"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="13">
         <v>1</v>
       </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F12" s="13"/>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E12" s="4"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12" s="13">
         <v>0</v>
@@ -822,74 +931,84 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F13" s="13"/>
+    <row r="13" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E13" s="4"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="13" t="s">
-        <v>15</v>
+      <c r="H13" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="I13" s="13">
         <v>0</v>
       </c>
-      <c r="J13" s="13">
-        <v>0.5</v>
+      <c r="J13" s="2">
+        <v>0.8</v>
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F14" s="13"/>
+    <row r="14" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E14" s="4"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I14" s="13">
         <v>0</v>
       </c>
       <c r="J14" s="13">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F15" s="13"/>
+    <row r="15" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E15" s="4"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I15" s="13">
         <v>0</v>
       </c>
       <c r="J15" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="6:15" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F16" s="13"/>
+    <row r="16" spans="5:21" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E16" s="4"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I16" s="13">
         <v>0</v>
       </c>
       <c r="J16" s="13">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E17" s="4"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
         <v>1.6</v>
       </c>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13">
-        <v>0</v>
-      </c>
-      <c r="J17" s="13"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F18" s="13"/>
+    <row r="18" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E18" s="4"/>
+      <c r="F18" s="22"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13">
@@ -898,8 +1017,9 @@
       <c r="J18" s="13"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F19" s="13"/>
+    <row r="19" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E19" s="4"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13">
@@ -908,8 +1028,9 @@
       <c r="J19" s="13"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F20" s="13"/>
+    <row r="20" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E20" s="4"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13">
@@ -918,8 +1039,9 @@
       <c r="J20" s="13"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F21" s="13"/>
+    <row r="21" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E21" s="4"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13">
@@ -928,8 +1050,9 @@
       <c r="J21" s="13"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F22" s="13"/>
+    <row r="22" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E22" s="4"/>
+      <c r="F22" s="22"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13">
@@ -938,8 +1061,9 @@
       <c r="J22" s="13"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F23" s="13"/>
+    <row r="23" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E23" s="4"/>
+      <c r="F23" s="22"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13">
@@ -948,8 +1072,9 @@
       <c r="J23" s="13"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F24" s="13"/>
+    <row r="24" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E24" s="4"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13">
@@ -958,8 +1083,9 @@
       <c r="J24" s="13"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F25" s="13"/>
+    <row r="25" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E25" s="4"/>
+      <c r="F25" s="22"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13">
@@ -968,8 +1094,9 @@
       <c r="J25" s="13"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F26" s="13"/>
+    <row r="26" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E26" s="4"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13">
@@ -978,8 +1105,9 @@
       <c r="J26" s="13"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F27" s="13"/>
+    <row r="27" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E27" s="4"/>
+      <c r="F27" s="22"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13">
@@ -988,8 +1116,9 @@
       <c r="J27" s="13"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F28" s="13"/>
+    <row r="28" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E28" s="4"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13">
@@ -998,8 +1127,9 @@
       <c r="J28" s="13"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F29" s="13"/>
+    <row r="29" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E29" s="4"/>
+      <c r="F29" s="22"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13">
@@ -1008,8 +1138,9 @@
       <c r="J29" s="13"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F30" s="13"/>
+    <row r="30" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E30" s="4"/>
+      <c r="F30" s="22"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13">
@@ -1018,8 +1149,9 @@
       <c r="J30" s="13"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F31" s="13"/>
+    <row r="31" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E31" s="4"/>
+      <c r="F31" s="22"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13">
@@ -1028,8 +1160,9 @@
       <c r="J31" s="13"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F32" s="13"/>
+    <row r="32" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E32" s="4"/>
+      <c r="F32" s="22"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13">
@@ -1038,8 +1171,9 @@
       <c r="J32" s="13"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F33" s="13"/>
+    <row r="33" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E33" s="4"/>
+      <c r="F33" s="22"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13">
@@ -1048,8 +1182,9 @@
       <c r="J33" s="13"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F34" s="13"/>
+    <row r="34" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E34" s="4"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13">
@@ -1058,8 +1193,9 @@
       <c r="J34" s="13"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F35" s="13"/>
+    <row r="35" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E35" s="4"/>
+      <c r="F35" s="22"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13">
@@ -1068,8 +1204,9 @@
       <c r="J35" s="13"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F36" s="13"/>
+    <row r="36" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E36" s="4"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13">
@@ -1078,8 +1215,9 @@
       <c r="J36" s="13"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F37" s="13"/>
+    <row r="37" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E37" s="4"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13">
@@ -1088,8 +1226,9 @@
       <c r="J37" s="13"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F38" s="13"/>
+    <row r="38" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E38" s="4"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13">
@@ -1098,8 +1237,9 @@
       <c r="J38" s="13"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F39" s="13"/>
+    <row r="39" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E39" s="4"/>
+      <c r="F39" s="22"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
       <c r="I39" s="13">
@@ -1108,8 +1248,9 @@
       <c r="J39" s="13"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F40" s="13"/>
+    <row r="40" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E40" s="4"/>
+      <c r="F40" s="22"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13">
@@ -1118,8 +1259,9 @@
       <c r="J40" s="13"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F41" s="13"/>
+    <row r="41" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E41" s="4"/>
+      <c r="F41" s="22"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13">
@@ -1128,8 +1270,9 @@
       <c r="J41" s="13"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F42" s="13"/>
+    <row r="42" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E42" s="4"/>
+      <c r="F42" s="22"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
       <c r="I42" s="13">
@@ -1138,8 +1281,9 @@
       <c r="J42" s="13"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F43" s="13"/>
+    <row r="43" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E43" s="4"/>
+      <c r="F43" s="22"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="13">
@@ -1148,8 +1292,9 @@
       <c r="J43" s="13"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F44" s="13"/>
+    <row r="44" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E44" s="4"/>
+      <c r="F44" s="22"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="13">
@@ -1158,8 +1303,9 @@
       <c r="J44" s="13"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F45" s="13"/>
+    <row r="45" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E45" s="4"/>
+      <c r="F45" s="22"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13">
@@ -1168,8 +1314,9 @@
       <c r="J45" s="13"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F46" s="13"/>
+    <row r="46" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E46" s="4"/>
+      <c r="F46" s="22"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
       <c r="I46" s="13">
@@ -1178,8 +1325,9 @@
       <c r="J46" s="13"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F47" s="13"/>
+    <row r="47" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E47" s="4"/>
+      <c r="F47" s="22"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13">
@@ -1188,8 +1336,9 @@
       <c r="J47" s="13"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F48" s="13"/>
+    <row r="48" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E48" s="4"/>
+      <c r="F48" s="22"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13">
@@ -1198,8 +1347,9 @@
       <c r="J48" s="13"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F49" s="13"/>
+    <row r="49" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E49" s="4"/>
+      <c r="F49" s="22"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13">
@@ -1208,8 +1358,9 @@
       <c r="J49" s="13"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F50" s="13"/>
+    <row r="50" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E50" s="4"/>
+      <c r="F50" s="22"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
       <c r="I50" s="13">
@@ -1218,8 +1369,9 @@
       <c r="J50" s="13"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F51" s="13"/>
+    <row r="51" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E51" s="4"/>
+      <c r="F51" s="22"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
       <c r="I51" s="13">
@@ -1228,8 +1380,9 @@
       <c r="J51" s="13"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F52" s="13"/>
+    <row r="52" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E52" s="4"/>
+      <c r="F52" s="22"/>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
       <c r="I52" s="13">
@@ -1238,8 +1391,9 @@
       <c r="J52" s="13"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F53" s="13"/>
+    <row r="53" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E53" s="4"/>
+      <c r="F53" s="22"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
       <c r="I53" s="13">
@@ -1248,8 +1402,9 @@
       <c r="J53" s="13"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F54" s="13"/>
+    <row r="54" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E54" s="4"/>
+      <c r="F54" s="22"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
       <c r="I54" s="13">
@@ -1258,8 +1413,9 @@
       <c r="J54" s="13"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F55" s="13"/>
+    <row r="55" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E55" s="4"/>
+      <c r="F55" s="22"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13">
@@ -1268,8 +1424,9 @@
       <c r="J55" s="13"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F56" s="13"/>
+    <row r="56" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E56" s="4"/>
+      <c r="F56" s="22"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
       <c r="I56" s="13">
@@ -1278,8 +1435,9 @@
       <c r="J56" s="13"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F57" s="13"/>
+    <row r="57" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E57" s="4"/>
+      <c r="F57" s="22"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
       <c r="I57" s="13">
@@ -1288,8 +1446,9 @@
       <c r="J57" s="13"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F58" s="13"/>
+    <row r="58" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E58" s="4"/>
+      <c r="F58" s="22"/>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
       <c r="I58" s="13">
@@ -1298,8 +1457,9 @@
       <c r="J58" s="13"/>
       <c r="K58" s="4"/>
     </row>
-    <row r="59" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F59" s="13"/>
+    <row r="59" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E59" s="4"/>
+      <c r="F59" s="22"/>
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
       <c r="I59" s="13">
@@ -1308,8 +1468,9 @@
       <c r="J59" s="13"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F60" s="13"/>
+    <row r="60" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E60" s="4"/>
+      <c r="F60" s="22"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
       <c r="I60" s="13">
@@ -1318,8 +1479,9 @@
       <c r="J60" s="13"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F61" s="13"/>
+    <row r="61" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E61" s="4"/>
+      <c r="F61" s="22"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13">
@@ -1328,8 +1490,9 @@
       <c r="J61" s="13"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F62" s="13"/>
+    <row r="62" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E62" s="4"/>
+      <c r="F62" s="22"/>
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13">
@@ -1338,8 +1501,9 @@
       <c r="J62" s="13"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F63" s="13"/>
+    <row r="63" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E63" s="4"/>
+      <c r="F63" s="22"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
       <c r="I63" s="13">
@@ -1348,8 +1512,9 @@
       <c r="J63" s="13"/>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F64" s="13"/>
+    <row r="64" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E64" s="4"/>
+      <c r="F64" s="22"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13">
@@ -1358,8 +1523,9 @@
       <c r="J64" s="13"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F65" s="13"/>
+    <row r="65" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E65" s="4"/>
+      <c r="F65" s="22"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
       <c r="I65" s="13">
@@ -1368,8 +1534,9 @@
       <c r="J65" s="13"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F66" s="13"/>
+    <row r="66" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E66" s="4"/>
+      <c r="F66" s="22"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13">
@@ -1378,8 +1545,9 @@
       <c r="J66" s="13"/>
       <c r="K66" s="4"/>
     </row>
-    <row r="67" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F67" s="13"/>
+    <row r="67" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E67" s="4"/>
+      <c r="F67" s="22"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
       <c r="I67" s="13">
@@ -1388,8 +1556,9 @@
       <c r="J67" s="13"/>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F68" s="13"/>
+    <row r="68" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E68" s="4"/>
+      <c r="F68" s="22"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
       <c r="I68" s="13">
@@ -1398,8 +1567,9 @@
       <c r="J68" s="13"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F69" s="13"/>
+    <row r="69" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E69" s="4"/>
+      <c r="F69" s="22"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13">
@@ -1408,8 +1578,9 @@
       <c r="J69" s="13"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F70" s="13"/>
+    <row r="70" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E70" s="4"/>
+      <c r="F70" s="22"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
       <c r="I70" s="13">
@@ -1418,8 +1589,9 @@
       <c r="J70" s="13"/>
       <c r="K70" s="4"/>
     </row>
-    <row r="71" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F71" s="13"/>
+    <row r="71" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E71" s="4"/>
+      <c r="F71" s="22"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
       <c r="I71" s="13">
@@ -1428,8 +1600,9 @@
       <c r="J71" s="13"/>
       <c r="K71" s="4"/>
     </row>
-    <row r="72" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F72" s="13"/>
+    <row r="72" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E72" s="4"/>
+      <c r="F72" s="22"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
       <c r="I72" s="13">
@@ -1438,8 +1611,9 @@
       <c r="J72" s="13"/>
       <c r="K72" s="4"/>
     </row>
-    <row r="73" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F73" s="13"/>
+    <row r="73" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E73" s="4"/>
+      <c r="F73" s="22"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
       <c r="I73" s="13">
@@ -1448,8 +1622,9 @@
       <c r="J73" s="13"/>
       <c r="K73" s="4"/>
     </row>
-    <row r="74" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F74" s="13"/>
+    <row r="74" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E74" s="4"/>
+      <c r="F74" s="22"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
       <c r="I74" s="13">
@@ -1458,8 +1633,9 @@
       <c r="J74" s="13"/>
       <c r="K74" s="4"/>
     </row>
-    <row r="75" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F75" s="13"/>
+    <row r="75" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E75" s="4"/>
+      <c r="F75" s="22"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
       <c r="I75" s="13">
@@ -1468,8 +1644,9 @@
       <c r="J75" s="13"/>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F76" s="13"/>
+    <row r="76" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E76" s="4"/>
+      <c r="F76" s="22"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
       <c r="I76" s="13">
@@ -1478,8 +1655,9 @@
       <c r="J76" s="13"/>
       <c r="K76" s="4"/>
     </row>
-    <row r="77" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F77" s="13"/>
+    <row r="77" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E77" s="4"/>
+      <c r="F77" s="22"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
       <c r="I77" s="13">
@@ -1488,8 +1666,9 @@
       <c r="J77" s="13"/>
       <c r="K77" s="4"/>
     </row>
-    <row r="78" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F78" s="13"/>
+    <row r="78" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E78" s="4"/>
+      <c r="F78" s="22"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
       <c r="I78" s="13">
@@ -1498,8 +1677,9 @@
       <c r="J78" s="13"/>
       <c r="K78" s="4"/>
     </row>
-    <row r="79" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F79" s="13"/>
+    <row r="79" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E79" s="4"/>
+      <c r="F79" s="22"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
       <c r="I79" s="13">
@@ -1508,8 +1688,9 @@
       <c r="J79" s="13"/>
       <c r="K79" s="4"/>
     </row>
-    <row r="80" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F80" s="13"/>
+    <row r="80" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E80" s="4"/>
+      <c r="F80" s="22"/>
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
       <c r="I80" s="13">
@@ -1518,8 +1699,9 @@
       <c r="J80" s="13"/>
       <c r="K80" s="4"/>
     </row>
-    <row r="81" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F81" s="13"/>
+    <row r="81" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E81" s="4"/>
+      <c r="F81" s="22"/>
       <c r="G81" s="13"/>
       <c r="H81" s="13"/>
       <c r="I81" s="13">
@@ -1528,8 +1710,9 @@
       <c r="J81" s="13"/>
       <c r="K81" s="4"/>
     </row>
-    <row r="82" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F82" s="13"/>
+    <row r="82" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E82" s="4"/>
+      <c r="F82" s="22"/>
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
       <c r="I82" s="13">
@@ -1538,8 +1721,9 @@
       <c r="J82" s="13"/>
       <c r="K82" s="4"/>
     </row>
-    <row r="83" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F83" s="13"/>
+    <row r="83" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E83" s="4"/>
+      <c r="F83" s="22"/>
       <c r="G83" s="13"/>
       <c r="H83" s="13"/>
       <c r="I83" s="13">
@@ -1548,8 +1732,9 @@
       <c r="J83" s="13"/>
       <c r="K83" s="4"/>
     </row>
-    <row r="84" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F84" s="13"/>
+    <row r="84" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E84" s="4"/>
+      <c r="F84" s="22"/>
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
       <c r="I84" s="13">
@@ -1558,8 +1743,9 @@
       <c r="J84" s="13"/>
       <c r="K84" s="4"/>
     </row>
-    <row r="85" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F85" s="13"/>
+    <row r="85" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E85" s="4"/>
+      <c r="F85" s="22"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
       <c r="I85" s="13">
@@ -1568,8 +1754,9 @@
       <c r="J85" s="13"/>
       <c r="K85" s="4"/>
     </row>
-    <row r="86" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F86" s="13"/>
+    <row r="86" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E86" s="4"/>
+      <c r="F86" s="22"/>
       <c r="G86" s="13"/>
       <c r="H86" s="13"/>
       <c r="I86" s="13">
@@ -1578,8 +1765,9 @@
       <c r="J86" s="13"/>
       <c r="K86" s="4"/>
     </row>
-    <row r="87" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F87" s="13"/>
+    <row r="87" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E87" s="4"/>
+      <c r="F87" s="22"/>
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
       <c r="I87" s="13">
@@ -1588,8 +1776,9 @@
       <c r="J87" s="13"/>
       <c r="K87" s="4"/>
     </row>
-    <row r="88" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F88" s="13"/>
+    <row r="88" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E88" s="4"/>
+      <c r="F88" s="22"/>
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
       <c r="I88" s="13">
@@ -1598,8 +1787,9 @@
       <c r="J88" s="13"/>
       <c r="K88" s="4"/>
     </row>
-    <row r="89" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F89" s="13"/>
+    <row r="89" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E89" s="4"/>
+      <c r="F89" s="22"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
       <c r="I89" s="13">
@@ -1608,8 +1798,9 @@
       <c r="J89" s="13"/>
       <c r="K89" s="4"/>
     </row>
-    <row r="90" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F90" s="13"/>
+    <row r="90" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E90" s="4"/>
+      <c r="F90" s="22"/>
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
       <c r="I90" s="13">
@@ -1618,8 +1809,9 @@
       <c r="J90" s="13"/>
       <c r="K90" s="4"/>
     </row>
-    <row r="91" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F91" s="13"/>
+    <row r="91" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E91" s="4"/>
+      <c r="F91" s="22"/>
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
       <c r="I91" s="13">
@@ -1628,8 +1820,9 @@
       <c r="J91" s="13"/>
       <c r="K91" s="4"/>
     </row>
-    <row r="92" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F92" s="13"/>
+    <row r="92" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E92" s="4"/>
+      <c r="F92" s="22"/>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
       <c r="I92" s="13">
@@ -1638,8 +1831,9 @@
       <c r="J92" s="13"/>
       <c r="K92" s="4"/>
     </row>
-    <row r="93" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F93" s="13"/>
+    <row r="93" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E93" s="4"/>
+      <c r="F93" s="22"/>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13">
@@ -1648,8 +1842,9 @@
       <c r="J93" s="13"/>
       <c r="K93" s="4"/>
     </row>
-    <row r="94" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F94" s="13"/>
+    <row r="94" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E94" s="4"/>
+      <c r="F94" s="22"/>
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
       <c r="I94" s="13">
@@ -1658,8 +1853,9 @@
       <c r="J94" s="13"/>
       <c r="K94" s="4"/>
     </row>
-    <row r="95" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F95" s="13"/>
+    <row r="95" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E95" s="4"/>
+      <c r="F95" s="22"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
       <c r="I95" s="13">
@@ -1668,8 +1864,9 @@
       <c r="J95" s="13"/>
       <c r="K95" s="4"/>
     </row>
-    <row r="96" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F96" s="13"/>
+    <row r="96" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E96" s="4"/>
+      <c r="F96" s="22"/>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
       <c r="I96" s="13">
@@ -1678,8 +1875,9 @@
       <c r="J96" s="13"/>
       <c r="K96" s="4"/>
     </row>
-    <row r="97" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F97" s="13"/>
+    <row r="97" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E97" s="4"/>
+      <c r="F97" s="22"/>
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
       <c r="I97" s="13">
@@ -1688,8 +1886,9 @@
       <c r="J97" s="13"/>
       <c r="K97" s="4"/>
     </row>
-    <row r="98" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F98" s="13"/>
+    <row r="98" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E98" s="4"/>
+      <c r="F98" s="22"/>
       <c r="G98" s="13"/>
       <c r="H98" s="13"/>
       <c r="I98" s="13">
@@ -1698,8 +1897,9 @@
       <c r="J98" s="13"/>
       <c r="K98" s="4"/>
     </row>
-    <row r="99" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1">
-      <c r="F99" s="13"/>
+    <row r="99" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="E99" s="4"/>
+      <c r="F99" s="22"/>
       <c r="G99" s="13"/>
       <c r="H99" s="13"/>
       <c r="I99" s="13">
@@ -1708,8 +1908,9 @@
       <c r="J99" s="13"/>
       <c r="K99" s="4"/>
     </row>
-    <row r="100" spans="6:11" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1">
-      <c r="F100" s="14"/>
+    <row r="100" spans="5:11" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1">
+      <c r="E100" s="4"/>
+      <c r="F100" s="23"/>
       <c r="G100" s="14"/>
       <c r="H100" s="14"/>
       <c r="I100" s="14">
@@ -1718,9 +1919,10 @@
       <c r="J100" s="14"/>
       <c r="K100" s="5"/>
     </row>
-    <row r="101" spans="6:11" ht="15" thickTop="1"/>
+    <row r="101" spans="5:11" ht="15.75" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>